<commit_message>
:construction: Add subject 8 data
</commit_message>
<xml_diff>
--- a/Responses.xlsx
+++ b/Responses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="86">
   <si>
     <t>Realism Rating</t>
   </si>
@@ -289,7 +289,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -934,9 +934,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="4" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
@@ -951,7 +951,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="37" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="3" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -961,7 +961,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="154">
+  <dxfs count="26">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -979,194 +979,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1395,1026 +1207,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2694,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T66"/>
+  <dimension ref="A1:V66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2722,9 +1514,11 @@
     <col min="18" max="18" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2761,8 +1555,12 @@
         <v>83</v>
       </c>
       <c r="T1" s="3"/>
+      <c r="U1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="39" t="s">
         <v>4</v>
       </c>
@@ -2823,8 +1621,14 @@
       <c r="T2" s="42" t="s">
         <v>1</v>
       </c>
+      <c r="U2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="42" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="37">
         <v>1</v>
       </c>
@@ -2841,7 +1645,7 @@
         <v>79</v>
       </c>
       <c r="F3" s="38">
-        <f>COUNTIF($G3:$DD3,"Yes")</f>
+        <f t="shared" ref="F3:F50" si="0">COUNTIF($G3:$DD3,"Yes")</f>
         <v>4</v>
       </c>
       <c r="G3" s="54">
@@ -2886,8 +1690,14 @@
       <c r="T3" s="27" t="s">
         <v>60</v>
       </c>
+      <c r="U3" s="54">
+        <v>2</v>
+      </c>
+      <c r="V3" s="27" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -2904,7 +1714,7 @@
         <v>79</v>
       </c>
       <c r="F4" s="38">
-        <f>COUNTIF($G4:$DD4,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G4" s="54">
@@ -2949,8 +1759,14 @@
       <c r="T4" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U4" s="54">
+        <v>1</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -2967,7 +1783,7 @@
         <v>79</v>
       </c>
       <c r="F5" s="38">
-        <f>COUNTIF($G5:$DD5,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G5" s="54">
@@ -3012,8 +1828,14 @@
       <c r="T5" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U5" s="54">
+        <v>2</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -3030,7 +1852,7 @@
         <v>79</v>
       </c>
       <c r="F6" s="38">
-        <f>COUNTIF($G6:$DD6,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G6" s="54">
@@ -3075,8 +1897,14 @@
       <c r="T6" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U6" s="54">
+        <v>3</v>
+      </c>
+      <c r="V6" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -3093,8 +1921,8 @@
         <v>79</v>
       </c>
       <c r="F7" s="38">
-        <f>COUNTIF($G7:$DD7,"Yes")</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="G7" s="54">
         <v>5</v>
@@ -3138,8 +1966,14 @@
       <c r="T7" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U7" s="54">
+        <v>1</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -3156,7 +1990,7 @@
         <v>79</v>
       </c>
       <c r="F8" s="38">
-        <f>COUNTIF($G8:$DD8,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G8" s="54">
@@ -3201,8 +2035,14 @@
       <c r="T8" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U8" s="54">
+        <v>2</v>
+      </c>
+      <c r="V8" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -3219,8 +2059,8 @@
         <v>79</v>
       </c>
       <c r="F9" s="38">
-        <f>COUNTIF($G9:$DD9,"Yes")</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="G9" s="54">
         <v>4</v>
@@ -3264,8 +2104,14 @@
       <c r="T9" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U9" s="54">
+        <v>2</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -3282,7 +2128,7 @@
         <v>79</v>
       </c>
       <c r="F10" s="38">
-        <f>COUNTIF($G10:$DD10,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G10" s="54">
@@ -3327,8 +2173,14 @@
       <c r="T10" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U10" s="54">
+        <v>2</v>
+      </c>
+      <c r="V10" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -3345,7 +2197,7 @@
         <v>79</v>
       </c>
       <c r="F11" s="38">
-        <f>COUNTIF($G11:$DD11,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G11" s="54">
@@ -3390,8 +2242,14 @@
       <c r="T11" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U11" s="54">
+        <v>3</v>
+      </c>
+      <c r="V11" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -3408,7 +2266,7 @@
         <v>79</v>
       </c>
       <c r="F12" s="38">
-        <f>COUNTIF($G12:$DD12,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G12" s="54">
@@ -3453,8 +2311,14 @@
       <c r="T12" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U12" s="54">
+        <v>3</v>
+      </c>
+      <c r="V12" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -3471,7 +2335,7 @@
         <v>79</v>
       </c>
       <c r="F13" s="38">
-        <f>COUNTIF($G13:$DD13,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G13" s="54">
@@ -3516,8 +2380,14 @@
       <c r="T13" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U13" s="54">
+        <v>3</v>
+      </c>
+      <c r="V13" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -3534,7 +2404,7 @@
         <v>79</v>
       </c>
       <c r="F14" s="38">
-        <f>COUNTIF($G14:$DD14,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G14" s="54">
@@ -3579,8 +2449,14 @@
       <c r="T14" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U14" s="54">
+        <v>2</v>
+      </c>
+      <c r="V14" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -3597,7 +2473,7 @@
         <v>79</v>
       </c>
       <c r="F15" s="38">
-        <f>COUNTIF($G15:$DD15,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15" s="54">
@@ -3642,8 +2518,14 @@
       <c r="T15" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U15" s="54">
+        <v>2</v>
+      </c>
+      <c r="V15" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -3660,7 +2542,7 @@
         <v>79</v>
       </c>
       <c r="F16" s="38">
-        <f>COUNTIF($G16:$DD16,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G16" s="54">
@@ -3705,8 +2587,14 @@
       <c r="T16" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U16" s="54">
+        <v>1</v>
+      </c>
+      <c r="V16" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -3723,7 +2611,7 @@
         <v>79</v>
       </c>
       <c r="F17" s="38">
-        <f>COUNTIF($G17:$DD17,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G17" s="54">
@@ -3768,8 +2656,14 @@
       <c r="T17" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U17" s="54">
+        <v>1</v>
+      </c>
+      <c r="V17" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -3786,8 +2680,8 @@
         <v>79</v>
       </c>
       <c r="F18" s="38">
-        <f>COUNTIF($G18:$DD18,"Yes")</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="G18" s="54">
         <v>2</v>
@@ -3831,8 +2725,14 @@
       <c r="T18" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U18" s="54">
+        <v>2</v>
+      </c>
+      <c r="V18" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -3849,7 +2749,7 @@
         <v>79</v>
       </c>
       <c r="F19" s="38">
-        <f>COUNTIF($G19:$DD19,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G19" s="54">
@@ -3894,8 +2794,14 @@
       <c r="T19" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U19" s="54">
+        <v>4</v>
+      </c>
+      <c r="V19" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -3912,7 +2818,7 @@
         <v>80</v>
       </c>
       <c r="F20" s="38">
-        <f>COUNTIF($G20:$DD20,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G20" s="54">
@@ -3957,8 +2863,14 @@
       <c r="T20" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U20" s="54">
+        <v>1</v>
+      </c>
+      <c r="V20" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -3975,7 +2887,7 @@
         <v>79</v>
       </c>
       <c r="F21" s="38">
-        <f>COUNTIF($G21:$DD21,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G21" s="54">
@@ -4020,8 +2932,14 @@
       <c r="T21" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U21" s="54">
+        <v>4</v>
+      </c>
+      <c r="V21" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -4038,7 +2956,7 @@
         <v>79</v>
       </c>
       <c r="F22" s="38">
-        <f>COUNTIF($G22:$DD22,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G22" s="54">
@@ -4083,8 +3001,14 @@
       <c r="T22" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U22" s="54">
+        <v>4</v>
+      </c>
+      <c r="V22" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -4101,7 +3025,7 @@
         <v>79</v>
       </c>
       <c r="F23" s="38">
-        <f>COUNTIF($G23:$DD23,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G23" s="54">
@@ -4146,8 +3070,14 @@
       <c r="T23" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U23" s="54">
+        <v>5</v>
+      </c>
+      <c r="V23" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -4164,7 +3094,7 @@
         <v>79</v>
       </c>
       <c r="F24" s="38">
-        <f>COUNTIF($G24:$DD24,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G24" s="54">
@@ -4209,8 +3139,14 @@
       <c r="T24" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U24" s="54">
+        <v>1</v>
+      </c>
+      <c r="V24" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -4227,7 +3163,7 @@
         <v>79</v>
       </c>
       <c r="F25" s="38">
-        <f>COUNTIF($G25:$DD25,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G25" s="54">
@@ -4272,8 +3208,14 @@
       <c r="T25" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U25" s="54">
+        <v>3</v>
+      </c>
+      <c r="V25" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -4290,7 +3232,7 @@
         <v>79</v>
       </c>
       <c r="F26" s="38">
-        <f>COUNTIF($G26:$DD26,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G26" s="54">
@@ -4335,8 +3277,14 @@
       <c r="T26" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U26" s="54">
+        <v>3</v>
+      </c>
+      <c r="V26" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -4353,7 +3301,7 @@
         <v>79</v>
       </c>
       <c r="F27" s="38">
-        <f>COUNTIF($G27:$DD27,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G27" s="54">
@@ -4398,8 +3346,14 @@
       <c r="T27" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U27" s="54">
+        <v>3</v>
+      </c>
+      <c r="V27" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -4416,7 +3370,7 @@
         <v>79</v>
       </c>
       <c r="F28" s="38">
-        <f>COUNTIF($G28:$DD28,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G28" s="54">
@@ -4461,8 +3415,14 @@
       <c r="T28" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U28" s="54">
+        <v>1</v>
+      </c>
+      <c r="V28" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -4479,8 +3439,8 @@
         <v>79</v>
       </c>
       <c r="F29" s="38">
-        <f>COUNTIF($G29:$DD29,"Yes")</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="G29" s="54">
         <v>2</v>
@@ -4524,8 +3484,14 @@
       <c r="T29" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U29" s="54">
+        <v>1</v>
+      </c>
+      <c r="V29" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -4542,7 +3508,7 @@
         <v>80</v>
       </c>
       <c r="F30" s="38">
-        <f>COUNTIF($G30:$DD30,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G30" s="54">
@@ -4587,8 +3553,14 @@
       <c r="T30" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U30" s="54">
+        <v>4</v>
+      </c>
+      <c r="V30" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -4605,7 +3577,7 @@
         <v>79</v>
       </c>
       <c r="F31" s="38">
-        <f>COUNTIF($G31:$DD31,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G31" s="54">
@@ -4650,8 +3622,14 @@
       <c r="T31" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U31" s="54">
+        <v>5</v>
+      </c>
+      <c r="V31" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>30</v>
       </c>
@@ -4668,7 +3646,7 @@
         <v>79</v>
       </c>
       <c r="F32" s="38">
-        <f>COUNTIF($G32:$DD32,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G32" s="54">
@@ -4713,8 +3691,14 @@
       <c r="T32" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U32" s="54">
+        <v>3</v>
+      </c>
+      <c r="V32" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -4731,7 +3715,7 @@
         <v>79</v>
       </c>
       <c r="F33" s="38">
-        <f>COUNTIF($G33:$DD33,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G33" s="54">
@@ -4776,8 +3760,14 @@
       <c r="T33" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U33" s="54">
+        <v>3</v>
+      </c>
+      <c r="V33" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -4794,7 +3784,7 @@
         <v>79</v>
       </c>
       <c r="F34" s="38">
-        <f>COUNTIF($G34:$DD34,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G34" s="54">
@@ -4839,8 +3829,14 @@
       <c r="T34" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U34" s="54">
+        <v>3</v>
+      </c>
+      <c r="V34" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -4857,7 +3853,7 @@
         <v>79</v>
       </c>
       <c r="F35" s="38">
-        <f>COUNTIF($G35:$DD35,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G35" s="54">
@@ -4902,8 +3898,14 @@
       <c r="T35" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U35" s="54">
+        <v>3</v>
+      </c>
+      <c r="V35" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -4920,8 +3922,8 @@
         <v>79</v>
       </c>
       <c r="F36" s="38">
-        <f>COUNTIF($G36:$DD36,"Yes")</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="G36" s="54">
         <v>2</v>
@@ -4965,8 +3967,14 @@
       <c r="T36" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U36" s="54">
+        <v>3</v>
+      </c>
+      <c r="V36" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -4983,8 +3991,8 @@
         <v>79</v>
       </c>
       <c r="F37" s="38">
-        <f>COUNTIF($G37:$DD37,"Yes")</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="G37" s="54">
         <v>4</v>
@@ -5028,8 +4036,14 @@
       <c r="T37" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U37" s="54">
+        <v>1</v>
+      </c>
+      <c r="V37" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -5046,8 +4060,8 @@
         <v>79</v>
       </c>
       <c r="F38" s="38">
-        <f>COUNTIF($G38:$DD38,"Yes")</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="G38" s="54">
         <v>4</v>
@@ -5091,8 +4105,14 @@
       <c r="T38" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U38" s="54">
+        <v>1</v>
+      </c>
+      <c r="V38" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -5109,7 +4129,7 @@
         <v>79</v>
       </c>
       <c r="F39" s="38">
-        <f>COUNTIF($G39:$DD39,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G39" s="54">
@@ -5154,8 +4174,14 @@
       <c r="T39" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U39" s="54">
+        <v>2</v>
+      </c>
+      <c r="V39" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -5172,7 +4198,7 @@
         <v>79</v>
       </c>
       <c r="F40" s="38">
-        <f>COUNTIF($G40:$DD40,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G40" s="54">
@@ -5217,8 +4243,14 @@
       <c r="T40" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U40" s="54">
+        <v>2</v>
+      </c>
+      <c r="V40" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -5235,7 +4267,7 @@
         <v>79</v>
       </c>
       <c r="F41" s="38">
-        <f>COUNTIF($G41:$DD41,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G41" s="54">
@@ -5280,8 +4312,14 @@
       <c r="T41" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U41" s="54">
+        <v>2</v>
+      </c>
+      <c r="V41" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
         <v>40</v>
       </c>
@@ -5298,7 +4336,7 @@
         <v>79</v>
       </c>
       <c r="F42" s="38">
-        <f>COUNTIF($G42:$DD42,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G42" s="54">
@@ -5343,8 +4381,14 @@
       <c r="T42" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U42" s="54">
+        <v>3</v>
+      </c>
+      <c r="V42" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -5361,7 +4405,7 @@
         <v>80</v>
       </c>
       <c r="F43" s="38">
-        <f>COUNTIF($G43:$DD43,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G43" s="54">
@@ -5406,8 +4450,14 @@
       <c r="T43" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U43" s="54">
+        <v>3</v>
+      </c>
+      <c r="V43" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -5424,7 +4474,7 @@
         <v>80</v>
       </c>
       <c r="F44" s="38">
-        <f>COUNTIF($G44:$DD44,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G44" s="54">
@@ -5469,8 +4519,14 @@
       <c r="T44" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U44" s="54">
+        <v>1</v>
+      </c>
+      <c r="V44" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -5487,7 +4543,7 @@
         <v>79</v>
       </c>
       <c r="F45" s="38">
-        <f>COUNTIF($G45:$DD45,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G45" s="54">
@@ -5532,8 +4588,14 @@
       <c r="T45" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U45" s="54">
+        <v>3</v>
+      </c>
+      <c r="V45" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -5550,7 +4612,7 @@
         <v>79</v>
       </c>
       <c r="F46" s="38">
-        <f>COUNTIF($G46:$DD46,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G46" s="54">
@@ -5595,8 +4657,14 @@
       <c r="T46" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U46" s="54">
+        <v>3</v>
+      </c>
+      <c r="V46" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -5613,7 +4681,7 @@
         <v>79</v>
       </c>
       <c r="F47" s="38">
-        <f>COUNTIF($G47:$DD47,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G47" s="54">
@@ -5658,8 +4726,14 @@
       <c r="T47" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U47" s="54">
+        <v>3</v>
+      </c>
+      <c r="V47" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -5676,7 +4750,7 @@
         <v>79</v>
       </c>
       <c r="F48" s="38">
-        <f>COUNTIF($G48:$DD48,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G48" s="54">
@@ -5721,8 +4795,14 @@
       <c r="T48" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="U48" s="54">
+        <v>2</v>
+      </c>
+      <c r="V48" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -5739,7 +4819,7 @@
         <v>79</v>
       </c>
       <c r="F49" s="38">
-        <f>COUNTIF($G49:$DD49,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G49" s="54">
@@ -5784,8 +4864,14 @@
       <c r="T49" s="11" t="s">
         <v>60</v>
       </c>
+      <c r="U49" s="54">
+        <v>3</v>
+      </c>
+      <c r="V49" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="50" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="12">
         <v>48</v>
       </c>
@@ -5802,7 +4888,7 @@
         <v>80</v>
       </c>
       <c r="F50" s="38">
-        <f>COUNTIF($G50:$DD50,"Yes")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G50" s="55">
@@ -5847,8 +4933,14 @@
       <c r="T50" s="13" t="s">
         <v>60</v>
       </c>
+      <c r="U50" s="55">
+        <v>3</v>
+      </c>
+      <c r="V50" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G51" s="57" t="s">
         <v>73</v>
       </c>
@@ -5898,8 +4990,15 @@
         <f>COUNTIF(T$3:T$50, "Yes")</f>
         <v>13</v>
       </c>
+      <c r="U51" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="V51" s="21">
+        <f>COUNTIF(V$3:V$50, "Yes")</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="52" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G52" s="50" t="s">
         <v>81</v>
       </c>
@@ -5949,8 +5048,15 @@
         <f>COUNTIFS(T$3:T$50, "Yes",  $E$3:$E$50, "Ok")</f>
         <v>10</v>
       </c>
+      <c r="U52" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="V52" s="51">
+        <f>COUNTIFS(V$3:V$50, "Yes",  $E$3:$E$50, "Ok")</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="53" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G53" s="18" t="s">
         <v>71</v>
       </c>
@@ -6000,8 +5106,15 @@
         <f>AVERAGE(S$3:S$50)</f>
         <v>3.1041666666666665</v>
       </c>
+      <c r="U53" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="V53" s="45">
+        <f>AVERAGE(U$3:U$50)</f>
+        <v>2.4583333333333335</v>
+      </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G54" s="33" t="s">
         <v>67</v>
       </c>
@@ -6051,8 +5164,15 @@
         <f>COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Corner") / COUNTIF($C$3:$C$50, "Corner")</f>
         <v>0.25</v>
       </c>
+      <c r="U54" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="V54" s="28">
+        <f>COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Corner") / COUNTIF($C$3:$C$50, "Corner")</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G55" s="23" t="s">
         <v>68</v>
       </c>
@@ -6102,8 +5222,15 @@
         <f>COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Edge") / COUNTIF($C$3:$C$50, "Edge")</f>
         <v>0.375</v>
       </c>
+      <c r="U55" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="V55" s="29">
+        <f>COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Edge") / COUNTIF($C$3:$C$50, "Edge")</f>
+        <v>0.125</v>
+      </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G56" s="23" t="s">
         <v>69</v>
       </c>
@@ -6153,8 +5280,15 @@
         <f>COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Center") / COUNTIF($C$3:$C$50, "Center")</f>
         <v>0.625</v>
       </c>
+      <c r="U56" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="V56" s="29">
+        <f>COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Center") / COUNTIF($C$3:$C$50, "Center")</f>
+        <v>0.25</v>
+      </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G57" s="24" t="s">
         <v>70</v>
       </c>
@@ -6204,8 +5338,15 @@
         <f>COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Normal") / COUNTIF($C$3:$C$50, "Normal")</f>
         <v>0.125</v>
       </c>
+      <c r="U57" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="V57" s="29">
+        <f>COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Normal") / COUNTIF($C$3:$C$50, "Normal")</f>
+        <v>0.16666666666666666</v>
+      </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G58" s="46" t="s">
         <v>81</v>
       </c>
@@ -6255,8 +5396,15 @@
         <f>COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Normal", $E$3:$E$50, "Ok") / COUNTIFS($C$3:$C$50, "Normal", $E$3:$E$50, "Ok")</f>
         <v>4.7619047619047616E-2</v>
       </c>
+      <c r="U58" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="V58" s="47">
+        <f>COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Normal", $E$3:$E$50, "Ok") / COUNTIFS($C$3:$C$50, "Normal", $E$3:$E$50, "Ok")</f>
+        <v>0.19047619047619047</v>
+      </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G59" s="46" t="s">
         <v>85</v>
       </c>
@@ -6306,8 +5454,15 @@
         <f>COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Normal", $E$3:$E$50, "Ok") / COUNTIF(T$3:T$50, "Yes")</f>
         <v>7.6923076923076927E-2</v>
       </c>
+      <c r="U59" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="V59" s="47">
+        <f>COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Normal", $E$3:$E$50, "Ok") / COUNTIF(V$3:V$50, "Yes")</f>
+        <v>0.5714285714285714</v>
+      </c>
     </row>
-    <row r="60" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G60" s="25" t="s">
         <v>72</v>
       </c>
@@ -6357,8 +5512,15 @@
         <f>(COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Corner") + COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Edge") + COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Center")) / SUMPRODUCT(COUNTIF($C$3:$C$50, {"Corner";"Edge";"Center"}))</f>
         <v>0.41666666666666669</v>
       </c>
+      <c r="U60" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="V60" s="30">
+        <f>(COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Corner") + COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Edge") + COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Center")) / SUMPRODUCT(COUNTIF($C$3:$C$50, {"Corner";"Edge";"Center"}))</f>
+        <v>0.125</v>
+      </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G61" s="26" t="s">
         <v>74</v>
       </c>
@@ -6408,8 +5570,15 @@
         <f>AVERAGEIFS(S$3:S$50, $C$3:$C$50, "Corner")</f>
         <v>3.25</v>
       </c>
+      <c r="U61" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="V61" s="45">
+        <f>AVERAGEIFS(U$3:U$50, $C$3:$C$50, "Corner")</f>
+        <v>2.75</v>
+      </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G62" s="20" t="s">
         <v>75</v>
       </c>
@@ -6459,8 +5628,15 @@
         <f>AVERAGEIFS(S$3:S$50, $C$3:$C$50, "Edge")</f>
         <v>2.375</v>
       </c>
+      <c r="U62" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="V62" s="43">
+        <f>AVERAGEIFS(U$3:U$50, $C$3:$C$50, "Edge")</f>
+        <v>2.375</v>
+      </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G63" s="20" t="s">
         <v>76</v>
       </c>
@@ -6510,8 +5686,15 @@
         <f>AVERAGEIFS(S$3:S$50, $C$3:$C$50, "Center")</f>
         <v>2.75</v>
       </c>
+      <c r="U63" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="V63" s="43">
+        <f>AVERAGEIFS(U$3:U$50, $C$3:$C$50, "Center")</f>
+        <v>2.375</v>
+      </c>
     </row>
-    <row r="64" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G64" s="18" t="s">
         <v>77</v>
       </c>
@@ -6561,8 +5744,15 @@
         <f>AVERAGEIFS(S$3:S$50, $C$3:$C$50, "Normal")</f>
         <v>3.4166666666666665</v>
       </c>
+      <c r="U64" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="V64" s="44">
+        <f>AVERAGEIFS(U$3:U$50, $C$3:$C$50, "Normal")</f>
+        <v>2.4166666666666665</v>
+      </c>
     </row>
-    <row r="65" spans="7:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:22" x14ac:dyDescent="0.3">
       <c r="G65" s="19" t="s">
         <v>84</v>
       </c>
@@ -6612,8 +5802,15 @@
         <f>(COUNTIFS(T$3:T$50,"Yes",$C$3:$C$50,"Corner")+COUNTIFS(T$3:T$50,"Yes",$C$3:$C$50,"Edge")+COUNTIFS(T$3:T$50,"Yes",$C$3:$C$50,"Center")+COUNTIFS(T$3:T$50,"No",$C$3:$C$50,"Normal"))/48</f>
         <v>0.64583333333333337</v>
       </c>
+      <c r="U65" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="V65" s="28">
+        <f>(COUNTIFS(V$3:V$50,"Yes",$C$3:$C$50,"Corner")+COUNTIFS(V$3:V$50,"Yes",$C$3:$C$50,"Edge")+COUNTIFS(V$3:V$50,"Yes",$C$3:$C$50,"Center")+COUNTIFS(V$3:V$50,"No",$C$3:$C$50,"Normal"))/48</f>
+        <v>0.47916666666666669</v>
+      </c>
     </row>
-    <row r="66" spans="7:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="7:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G66" s="18" t="s">
         <v>81</v>
       </c>
@@ -6663,32 +5860,39 @@
         <f>(COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Corner", $E$3:$E$50, "Ok") + COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Edge", $E$3:$E$50, "Ok") + COUNTIFS(T$3:T$50, "Yes", $C$3:$C$50, "Center", $E$3:$E$50, "Ok") + COUNTIFS(T$3:T$50, "No", $C$3:$C$50, "Normal", $E$3:$E$50, "Ok"))/COUNTIF($E$3:$E$50,"Ok")</f>
         <v>0.67441860465116277</v>
       </c>
+      <c r="U66" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="V66" s="30">
+        <f>(COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Corner", $E$3:$E$50, "Ok") + COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Edge", $E$3:$E$50, "Ok") + COUNTIFS(V$3:V$50, "Yes", $C$3:$C$50, "Center", $E$3:$E$50, "Ok") + COUNTIFS(V$3:V$50, "No", $C$3:$C$50, "Normal", $E$3:$E$50, "Ok"))/COUNTIF($E$3:$E$50,"Ok")</f>
+        <v>0.46511627906976744</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:D1 C61:D1048576 C51:D56 C2:C50">
-    <cfRule type="cellIs" dxfId="21" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="118" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="119" operator="equal">
       <formula>"Center"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="120" operator="equal">
       <formula>"Edge"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="121" operator="equal">
       <formula>"Corner"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="17" priority="103" operator="containsText" text="dense">
+    <cfRule type="containsText" dxfId="19" priority="114" operator="containsText" text="dense">
       <formula>NOT(ISERROR(SEARCH("dense",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="104" operator="containsText" text="sparse">
+    <cfRule type="containsText" dxfId="18" priority="115" operator="containsText" text="sparse">
       <formula>NOT(ISERROR(SEARCH("sparse",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54:H56 J54:J56 L54:L56 N54:N56 P54:P56 R54:R56 R60 P60 N60 L60 J60 H60">
-    <cfRule type="dataBar" priority="80">
+    <cfRule type="dataBar" priority="91">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6702,7 +5906,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H59">
-    <cfRule type="dataBar" priority="78">
+    <cfRule type="dataBar" priority="89">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6716,7 +5920,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R57:R58">
-    <cfRule type="dataBar" priority="73">
+    <cfRule type="dataBar" priority="84">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6730,7 +5934,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:J58">
-    <cfRule type="dataBar" priority="77">
+    <cfRule type="dataBar" priority="88">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6744,7 +5948,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57:L58">
-    <cfRule type="dataBar" priority="76">
+    <cfRule type="dataBar" priority="87">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6758,7 +5962,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57:N58">
-    <cfRule type="dataBar" priority="75">
+    <cfRule type="dataBar" priority="86">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6772,7 +5976,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P57:P58">
-    <cfRule type="dataBar" priority="74">
+    <cfRule type="dataBar" priority="85">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6786,7 +5990,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F50">
-    <cfRule type="iconSet" priority="72">
+    <cfRule type="iconSet" priority="83">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -6795,23 +5999,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E50">
-    <cfRule type="cellIs" dxfId="15" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="81" operator="equal">
       <formula>"Ok"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="82" operator="equal">
       <formula>"Glitched"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T50">
-    <cfRule type="expression" dxfId="13" priority="58">
+    <cfRule type="expression" dxfId="15" priority="69">
       <formula>IF(OR(AND(T3="Yes",$C3&lt;&gt;"Normal"),AND(T3="No",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="68">
+    <cfRule type="expression" dxfId="14" priority="79">
       <formula>IF(OR(AND(T3="No",$C3&lt;&gt;"Normal"),AND(T3="Yes",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T54:T56 T60">
-    <cfRule type="dataBar" priority="60">
+    <cfRule type="dataBar" priority="71">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6825,7 +6029,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T57:T58">
-    <cfRule type="dataBar" priority="59">
+    <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6839,55 +6043,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R50">
-    <cfRule type="expression" dxfId="11" priority="56">
+    <cfRule type="expression" dxfId="13" priority="67">
       <formula>IF(OR(AND(R3="Yes",$C3&lt;&gt;"Normal"),AND(R3="No",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="57">
+    <cfRule type="expression" dxfId="12" priority="68">
       <formula>IF(OR(AND(R3="No",$C3&lt;&gt;"Normal"),AND(R3="Yes",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P50">
-    <cfRule type="expression" dxfId="9" priority="54">
+    <cfRule type="expression" dxfId="11" priority="65">
       <formula>IF(OR(AND(P3="Yes",$C3&lt;&gt;"Normal"),AND(P3="No",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="55">
+    <cfRule type="expression" dxfId="10" priority="66">
       <formula>IF(OR(AND(P3="No",$C3&lt;&gt;"Normal"),AND(P3="Yes",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N50">
-    <cfRule type="expression" dxfId="7" priority="52">
+    <cfRule type="expression" dxfId="9" priority="63">
       <formula>IF(OR(AND(N3="Yes",$C3&lt;&gt;"Normal"),AND(N3="No",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="53">
+    <cfRule type="expression" dxfId="8" priority="64">
       <formula>IF(OR(AND(N3="No",$C3&lt;&gt;"Normal"),AND(N3="Yes",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L50">
-    <cfRule type="expression" dxfId="5" priority="50">
+    <cfRule type="expression" dxfId="7" priority="61">
       <formula>IF(OR(AND(L3="Yes",$C3&lt;&gt;"Normal"),AND(L3="No",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="51">
+    <cfRule type="expression" dxfId="6" priority="62">
       <formula>IF(OR(AND(L3="No",$C3&lt;&gt;"Normal"),AND(L3="Yes",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J50">
-    <cfRule type="expression" dxfId="3" priority="48">
+    <cfRule type="expression" dxfId="5" priority="59">
       <formula>IF(OR(AND(J3="Yes",$C3&lt;&gt;"Normal"),AND(J3="No",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="49">
+    <cfRule type="expression" dxfId="4" priority="60">
       <formula>IF(OR(AND(J3="No",$C3&lt;&gt;"Normal"),AND(J3="Yes",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H50">
-    <cfRule type="expression" dxfId="1" priority="46">
+    <cfRule type="expression" dxfId="3" priority="57">
       <formula>IF(OR(AND(H3="Yes",$C3&lt;&gt;"Normal"),AND(H3="No",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="47">
+    <cfRule type="expression" dxfId="2" priority="58">
       <formula>IF(OR(AND(H3="No",$C3&lt;&gt;"Normal"),AND(H3="Yes",$C3="Normal")),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61:H64">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="3"/>
@@ -6899,7 +6103,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G50">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="3"/>
@@ -6911,7 +6115,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="percentile" val="50"/>
@@ -6923,7 +6127,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J53">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="percentile" val="50"/>
@@ -6935,7 +6139,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="percentile" val="50"/>
@@ -6947,6 +6151,126 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N53">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P53">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R53">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T53">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I50">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K50">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M50">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O50">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q50">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S50">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J61:J64">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -6958,7 +6282,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P53">
+  <conditionalFormatting sqref="L61:L64">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -6970,7 +6294,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R53">
+  <conditionalFormatting sqref="N61:N64">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -6982,7 +6306,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T53">
+  <conditionalFormatting sqref="P61:P64">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -6994,7 +6318,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I50">
+  <conditionalFormatting sqref="R61:R64">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -7006,7 +6330,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K50">
+  <conditionalFormatting sqref="T61:T64">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -7018,128 +6342,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M50">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O50">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q50">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S50">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J61:J64">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L61:L64">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N61:N64">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P61:P64">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R61:R64">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T61:T64">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J59">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7153,7 +6357,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7167,7 +6371,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N59">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7181,7 +6385,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P59">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7195,7 +6399,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R59">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7209,7 +6413,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T59">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -7220,6 +6424,92 @@
           <x14:id>{3D5E0874-9168-4D29-B25D-3A0F87C0BB19}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V50">
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>IF(OR(AND(V3="Yes",$C3&lt;&gt;"Normal"),AND(V3="No",$C3="Normal")),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="11">
+      <formula>IF(OR(AND(V3="No",$C3&lt;&gt;"Normal"),AND(V3="Yes",$C3="Normal")),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V54:V56 V60">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{99248665-9A6D-4AFF-95B0-4D8C6755FDC8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V57:V58">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8B9E89A9-4DA4-4396-BFB9-72756A62D660}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V59">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D89520B7-6077-4D37-B7D3-92DAA78D8216}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3:U50">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V53">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V61:V64">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7478,6 +6768,55 @@
           </x14:cfRule>
           <xm:sqref>T59</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{99248665-9A6D-4AFF-95B0-4D8C6755FDC8}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>V54:V56 V60</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8B9E89A9-4DA4-4396-BFB9-72756A62D660}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>V57:V58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D89520B7-6077-4D37-B7D3-92DAA78D8216}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>V59</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>